<commit_message>
support duplicates - added a `status` column to the `data` sheet
</commit_message>
<xml_diff>
--- a/sample_output.xlsx
+++ b/sample_output.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="347" windowWidth="7049" windowHeight="2269"/>
+    <workbookView xWindow="0" yWindow="347" windowWidth="7049" windowHeight="2269" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="recon" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>column1</t>
   </si>
@@ -67,13 +67,43 @@
   </si>
   <si>
     <t>note</t>
+  </si>
+  <si>
+    <t>LHS</t>
+  </si>
+  <si>
+    <t>RHS</t>
+  </si>
+  <si>
+    <t>this recon corresponds to the following inputs (the order of the rows does not matter)</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>recon</t>
+  </si>
+  <si>
+    <t>duplicated key</t>
+  </si>
+  <si>
+    <t>muchachos</t>
+  </si>
+  <si>
+    <t>duplicate</t>
+  </si>
+  <si>
+    <t>population break</t>
+  </si>
+  <si>
+    <t>missing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +115,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -128,13 +165,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -143,15 +181,10 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
+          <fgColor rgb="FF00B0F0"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -160,6 +193,11 @@
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -186,12 +224,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:C9"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:D10"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="key"/>
     <tableColumn id="2" name="input"/>
-    <tableColumn id="3" name="column1" dataDxfId="2"/>
+    <tableColumn id="4" name="status"/>
+    <tableColumn id="3" name="column1" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -462,7 +501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -485,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="b">
-        <f>EXACT(data!C2,data!C3)</f>
+        <f>EXACT(data!D2,data!D3)</f>
         <v>1</v>
       </c>
     </row>
@@ -495,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="b">
-        <f>EXACT(data!C4,data!C5)</f>
+        <f>EXACT(data!D4,data!D5)</f>
         <v>0</v>
       </c>
     </row>
@@ -505,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="b">
-        <f>EXACT(data!C6,data!C7)</f>
+        <f>EXACT(data!D6,data!D7)</f>
         <v>1</v>
       </c>
     </row>
@@ -520,19 +559,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" customWidth="1"/>
-    <col min="3" max="3" width="9.3984375" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -540,76 +581,97 @@
         <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -617,22 +679,139 @@
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C10" s="3"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more clarifications to the sample output .xls
</commit_message>
<xml_diff>
--- a/sample_output.xlsx
+++ b/sample_output.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="347" windowWidth="7049" windowHeight="2269" activeTab="1"/>
+    <workbookView xWindow="671" yWindow="347" windowWidth="7049" windowHeight="2269" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="recon" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>recon</t>
-  </si>
-  <si>
     <t>duplicated key</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>missing</t>
+  </si>
+  <si>
+    <t>common</t>
   </si>
 </sst>
 </file>
@@ -177,15 +177,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B0F0"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -224,13 +216,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:D10"/>
   <tableColumns count="4">
     <tableColumn id="1" name="key"/>
     <tableColumn id="2" name="input"/>
     <tableColumn id="4" name="status"/>
-    <tableColumn id="3" name="column1" dataDxfId="1"/>
+    <tableColumn id="3" name="column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -562,7 +554,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -595,7 +587,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -609,7 +601,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -623,7 +615,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -637,7 +629,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>3</v>
@@ -651,7 +643,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>13</v>
@@ -665,7 +657,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>13</v>
@@ -679,7 +671,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>3</v>
@@ -693,10 +685,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -707,7 +699,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>2</v>
@@ -784,7 +776,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -799,18 +791,18 @@
         <v>2</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed the names of the columns on the data sheet
</commit_message>
<xml_diff>
--- a/sample_output.xlsx
+++ b/sample_output.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="671" yWindow="347" windowWidth="7049" windowHeight="2269" activeTab="1"/>
+    <workbookView xWindow="671" yWindow="694" windowWidth="7049" windowHeight="2269" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="recon" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>mundo</t>
   </si>
   <si>
-    <t>input</t>
-  </si>
-  <si>
     <t>lhs</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>this recon corresponds to the following inputs (the order of the rows does not matter)</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>duplicated key</t>
   </si>
   <si>
@@ -97,6 +91,12 @@
   </si>
   <si>
     <t>common</t>
+  </si>
+  <si>
+    <t>~InputName~</t>
+  </si>
+  <si>
+    <t>~RecordType~</t>
   </si>
 </sst>
 </file>
@@ -220,8 +220,8 @@
   <autoFilter ref="A1:D10"/>
   <tableColumns count="4">
     <tableColumn id="1" name="key"/>
-    <tableColumn id="2" name="input"/>
-    <tableColumn id="4" name="status"/>
+    <tableColumn id="2" name="~InputName~"/>
+    <tableColumn id="4" name="~RecordType~"/>
     <tableColumn id="3" name="column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -504,7 +504,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -554,26 +554,27 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" customWidth="1"/>
+    <col min="3" max="3" width="15.53125" customWidth="1"/>
     <col min="4" max="4" width="9.3984375" customWidth="1"/>
     <col min="7" max="7" width="12.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
@@ -581,30 +582,30 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -612,10 +613,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -626,10 +627,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>3</v>
@@ -637,41 +638,41 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>3</v>
@@ -679,27 +680,27 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>2</v>
@@ -707,26 +708,26 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>0</v>
@@ -734,16 +735,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
       <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
         <v>9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -762,47 +763,47 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
       <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
         <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>